<commit_message>
conf scheduling: fix changing the configuration tab should not crash the read + fix rewards shouldn't undo penalty orange coloring
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -20,8 +20,83 @@
 </workbook>
 </file>
 
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t>S028: Securing scalable Hibernate
+  Chad Poe
+  PINNED BY USER</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t>S028: Securing scalable Hibernate
+  Chad Poe
+  PINNED BY USER</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C45" authorId="0">
+      <text>
+        <t>S028: Securing scalable Hibernate
+  Chad Poe
+  PINNED BY USER</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t>S028: Securing scalable Hibernate
+  Chad Poe
+  PINNED BY USER</t>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <t>S028: Securing scalable Hibernate
+  Chad Poe
+  PINNED BY USER</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6300" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6351" uniqueCount="479">
   <si>
     <t>Conference name</t>
   </si>
@@ -1776,6 +1851,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1928,26 +2006,60 @@
       <c r="A3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+      <c r="D3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -1957,6 +2069,7 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -16743,6 +16856,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17508,11 +17624,15 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21917,11 +22037,15 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22074,51 +22198,119 @@
       <c r="A3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+      <c r="D3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -22128,11 +22320,15 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
conf scheduling: audienceTypes (plural)
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6640" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6641" uniqueCount="528">
   <si>
     <t>Conference name</t>
   </si>
@@ -681,7 +681,7 @@
     <t>Sector tags</t>
   </si>
   <si>
-    <t>Audience type</t>
+    <t>Audience types</t>
   </si>
   <si>
     <t>Audience level</t>
@@ -1687,6 +1687,9 @@
   </si>
   <si>
     <t>Usable sessions</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
   <si>
     <t>S073: Grok distributed Tensorflow
@@ -1703,6 +1706,9 @@
   </si>
   <si>
     <t>Sector tag</t>
+  </si>
+  <si>
+    <t>Audience type</t>
   </si>
   <si>
     <t>1</t>
@@ -2313,7 +2319,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -2477,7 +2483,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>182</v>
+        <v>524</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -2542,7 +2548,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -2760,13 +2766,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -2925,7 +2931,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -2990,7 +2996,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -18278,6 +18284,24 @@
       </c>
       <c r="E5" s="2" t="n">
         <v>96.0</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>180.0</v>
       </c>
     </row>
   </sheetData>
@@ -18466,7 +18490,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -19156,7 +19180,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -21050,7 +21074,7 @@
         <v>65</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>65</v>
@@ -23569,7 +23593,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -23634,7 +23658,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -23693,7 +23717,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
conf scheduling: TalkType concept + value range from entity to improve speed
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -3580,7 +3580,7 @@
       <c r="C3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -3589,7 +3589,7 @@
       <c r="F3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -3598,7 +3598,7 @@
       <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -3607,7 +3607,7 @@
       <c r="L3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -3616,7 +3616,7 @@
       <c r="O3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -3625,7 +3625,7 @@
       <c r="R3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T3" s="2" t="s">
@@ -3645,7 +3645,7 @@
       <c r="C4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -3654,7 +3654,7 @@
       <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -3663,7 +3663,7 @@
       <c r="I4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -3672,7 +3672,7 @@
       <c r="L4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -3681,7 +3681,7 @@
       <c r="O4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q4" s="2" t="s">
@@ -3690,7 +3690,7 @@
       <c r="R4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T4" s="2" t="s">
@@ -3710,7 +3710,7 @@
       <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -3719,7 +3719,7 @@
       <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -3728,7 +3728,7 @@
       <c r="I5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -3737,7 +3737,7 @@
       <c r="L5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -3746,7 +3746,7 @@
       <c r="O5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -3755,7 +3755,7 @@
       <c r="R5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T5" s="2" t="s">
@@ -3775,7 +3775,7 @@
       <c r="C6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -3784,7 +3784,7 @@
       <c r="F6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -3793,7 +3793,7 @@
       <c r="I6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -3802,7 +3802,7 @@
       <c r="L6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -3811,7 +3811,7 @@
       <c r="O6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q6" s="2" t="s">
@@ -3820,7 +3820,7 @@
       <c r="R6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T6" s="2" t="s">
@@ -3843,55 +3843,55 @@
       <c r="D7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="K7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O7" s="3" t="s">
+      <c r="N7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R7" s="3" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="U7" s="3" t="s">
+      <c r="T7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       <c r="C8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -3914,7 +3914,7 @@
       <c r="F8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -3923,7 +3923,7 @@
       <c r="I8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -3932,7 +3932,7 @@
       <c r="L8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N8" s="2" t="s">
@@ -3941,7 +3941,7 @@
       <c r="O8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="2" t="s">
@@ -3950,7 +3950,7 @@
       <c r="R8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T8" s="2" t="s">
@@ -3970,7 +3970,7 @@
       <c r="C9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -3979,7 +3979,7 @@
       <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -3988,7 +3988,7 @@
       <c r="I9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -3997,7 +3997,7 @@
       <c r="L9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -4006,7 +4006,7 @@
       <c r="O9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q9" s="2" t="s">
@@ -4015,7 +4015,7 @@
       <c r="R9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T9" s="2" t="s">
@@ -4035,7 +4035,7 @@
       <c r="C10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -4044,7 +4044,7 @@
       <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -4053,7 +4053,7 @@
       <c r="I10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -4062,7 +4062,7 @@
       <c r="L10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -4071,7 +4071,7 @@
       <c r="O10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q10" s="2" t="s">
@@ -4080,7 +4080,7 @@
       <c r="R10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="S10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T10" s="2" t="s">
@@ -4100,7 +4100,7 @@
       <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -4109,7 +4109,7 @@
       <c r="F11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -4118,7 +4118,7 @@
       <c r="I11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -4127,7 +4127,7 @@
       <c r="L11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N11" s="2" t="s">
@@ -4136,7 +4136,7 @@
       <c r="O11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="Q11" s="2" t="s">
@@ -4145,7 +4145,7 @@
       <c r="R11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="T11" s="2" t="s">
@@ -4168,55 +4168,55 @@
       <c r="D12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="K12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="N12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R12" s="3" t="s">
+      <c r="Q12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="U12" s="3" t="s">
+      <c r="T12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="2" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
conf scheduling: increase weight on content conflict and enable some other score rules
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -1924,7 +1924,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -1946,7 +1946,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -1968,7 +1968,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1990,7 +1990,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
@@ -2001,7 +2001,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
@@ -2012,7 +2012,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -2023,7 +2023,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>24</v>
@@ -2034,7 +2034,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -2045,7 +2045,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>30</v>
@@ -2056,7 +2056,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>28</v>
@@ -2067,7 +2067,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Extract XLSX common code from conference scheduling example
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -11,14 +11,16 @@
     <sheet name="Rooms" r:id="rId5" sheetId="3"/>
     <sheet name="Speakers" r:id="rId6" sheetId="4"/>
     <sheet name="Talks" r:id="rId7" sheetId="5"/>
-    <sheet name="Score view" r:id="rId8" sheetId="6"/>
+    <sheet name="Infeasible view" r:id="rId8" sheetId="6"/>
     <sheet name="Rooms view" r:id="rId9" sheetId="7"/>
     <sheet name="Speakers view" r:id="rId10" sheetId="8"/>
     <sheet name="Theme tracks view" r:id="rId11" sheetId="9"/>
     <sheet name="Sectors view" r:id="rId12" sheetId="10"/>
-    <sheet name="Audience type view" r:id="rId13" sheetId="11"/>
-    <sheet name="Audience level view" r:id="rId14" sheetId="12"/>
+    <sheet name="Audience types view" r:id="rId13" sheetId="11"/>
+    <sheet name="Audience levels view" r:id="rId14" sheetId="12"/>
     <sheet name="Contents view" r:id="rId15" sheetId="13"/>
+    <sheet name="Languages view" r:id="rId16" sheetId="14"/>
+    <sheet name="Score view" r:id="rId17" sheetId="15"/>
   </sheets>
 </workbook>
 </file>
@@ -31,9 +33,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -48,9 +51,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -65,9 +69,28 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -82,9 +105,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -99,9 +123,10 @@
   <commentList>
     <comment ref="C34" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -116,16 +141,18 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
     <comment ref="C4" authorId="0">
       <text>
-        <t>S073: Grok distributed Tensorflow
-  Beth King
-  PINNED BY USER</t>
+        <t xml:space="preserve">S073: Grok distributed Tensorflow
+    Beth King
+PINNED BY USER
+</t>
       </text>
     </comment>
   </commentList>
@@ -133,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6641" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6703" uniqueCount="531">
   <si>
     <t>Conference name</t>
   </si>
@@ -1718,6 +1745,15 @@
   </si>
   <si>
     <t>S073 (level 1)</t>
+  </si>
+  <si>
+    <t>Constraint match</t>
+  </si>
+  <si>
+    <t>Match score</t>
+  </si>
+  <si>
+    <t>Total score</t>
   </si>
 </sst>
 </file>
@@ -1829,6 +1865,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
@@ -3056,6 +3100,273 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" ht="15.0" customHeight="true">
+      <c r="A3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="16.8125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.296875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.08203125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18301,7 +18612,7 @@
         <v>10.0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>180.0</v>
+        <v>108.0</v>
       </c>
     </row>
   </sheetData>
@@ -18482,7 +18793,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" ht="60.0" customHeight="true">
+    <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
@@ -18541,7 +18852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" ht="60.0" customHeight="true">
+    <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -18600,7 +18911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" ht="60.0" customHeight="true">
+    <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
@@ -18659,7 +18970,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" ht="60.0" customHeight="true">
+    <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -18718,7 +19029,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" ht="60.0" customHeight="true">
+    <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -18777,7 +19088,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" ht="60.0" customHeight="true">
+    <row r="8" ht="45.0" customHeight="true">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -18836,7 +19147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" ht="60.0" customHeight="true">
+    <row r="9" ht="45.0" customHeight="true">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -18895,7 +19206,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" ht="60.0" customHeight="true">
+    <row r="10" ht="45.0" customHeight="true">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -18954,7 +19265,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" ht="60.0" customHeight="true">
+    <row r="11" ht="45.0" customHeight="true">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -19013,7 +19324,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" ht="60.0" customHeight="true">
+    <row r="12" ht="45.0" customHeight="true">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -19099,24 +19410,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="11.75390625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.0" customWidth="true"/>
+    <col min="3" max="3" width="20.0" customWidth="true"/>
+    <col min="4" max="4" width="20.0" customWidth="true"/>
+    <col min="5" max="5" width="20.0" customWidth="true"/>
+    <col min="6" max="6" width="20.0" customWidth="true"/>
+    <col min="7" max="7" width="20.0" customWidth="true"/>
+    <col min="8" max="8" width="20.0" customWidth="true"/>
+    <col min="9" max="9" width="20.0" customWidth="true"/>
+    <col min="10" max="10" width="20.0" customWidth="true"/>
+    <col min="11" max="11" width="20.0" customWidth="true"/>
+    <col min="12" max="12" width="20.0" customWidth="true"/>
+    <col min="13" max="13" width="20.0" customWidth="true"/>
+    <col min="14" max="14" width="20.0" customWidth="true"/>
+    <col min="15" max="15" width="20.0" customWidth="true"/>
+    <col min="16" max="16" width="20.0" customWidth="true"/>
+    <col min="17" max="17" width="20.0" customWidth="true"/>
+    <col min="18" max="18" width="20.0" customWidth="true"/>
+    <col min="19" max="19" width="20.0" customWidth="true"/>
+    <col min="20" max="20" width="20.0" customWidth="true"/>
+    <col min="21" max="21" width="20.0" customWidth="true"/>
+    <col min="22" max="22" width="20.0" customWidth="true"/>
+    <col min="23" max="23" width="20.0" customWidth="true"/>
+    <col min="24" max="24" width="20.0" customWidth="true"/>
+    <col min="25" max="25" width="20.0" customWidth="true"/>
+    <col min="26" max="26" width="20.0" customWidth="true"/>
+    <col min="27" max="27" width="20.0" customWidth="true"/>
+    <col min="28" max="28" width="20.0" customWidth="true"/>
+    <col min="29" max="29" width="20.0" customWidth="true"/>
+    <col min="30" max="30" width="20.0" customWidth="true"/>
+    <col min="31" max="31" width="20.0" customWidth="true"/>
+    <col min="32" max="32" width="20.0" customWidth="true"/>
+    <col min="33" max="33" width="20.0" customWidth="true"/>
+    <col min="34" max="34" width="20.0" customWidth="true"/>
+    <col min="35" max="35" width="20.0" customWidth="true"/>
+    <col min="36" max="36" width="20.0" customWidth="true"/>
+    <col min="37" max="37" width="20.0" customWidth="true"/>
+    <col min="38" max="38" width="20.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Fix typos and drools warning
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -225,40 +225,40 @@
     <t>Soft reward per 2 talks that have the same timeslot and a different language</t>
   </si>
   <si>
-    <t>Speaker preferred timeslot tag</t>
+    <t>Speaker preferred timeslot tags</t>
   </si>
   <si>
     <t>Soft penalty per missing preferred tag in a talk's timeslot</t>
   </si>
   <si>
-    <t>Speaker undesired timeslot tag</t>
+    <t>Speaker undesired timeslot tags</t>
   </si>
   <si>
     <t>Soft penalty per undesired tag in a talk's timeslot</t>
   </si>
   <si>
-    <t>Talk preferred timeslot tag</t>
-  </si>
-  <si>
-    <t>Talk undesired timeslot tag</t>
-  </si>
-  <si>
-    <t>Speaker preferred room tag</t>
+    <t>Talk preferred timeslot tags</t>
+  </si>
+  <si>
+    <t>Talk undesired timeslot tags</t>
+  </si>
+  <si>
+    <t>Speaker preferred room tags</t>
   </si>
   <si>
     <t>Soft penalty per missing preferred tag in a talk's room</t>
   </si>
   <si>
-    <t>Speaker undesired room tag</t>
+    <t>Speaker undesired room tags</t>
   </si>
   <si>
     <t>Soft penalty per undesired tag in a talk's room</t>
   </si>
   <si>
-    <t>Talk preferred room tag</t>
-  </si>
-  <si>
-    <t>Talk undesired room tag</t>
+    <t>Talk preferred room tags</t>
+  </si>
+  <si>
+    <t>Talk undesired room tags</t>
   </si>
   <si>
     <t>Same day talks</t>
@@ -309,43 +309,43 @@
     <t>Hard penalty per pair of talks with the same speaker in overlapping timeslots</t>
   </si>
   <si>
-    <t>Speaker required timeslot tag</t>
+    <t>Speaker required timeslot tags</t>
   </si>
   <si>
     <t>Hard penalty per missing required tag in a talk's timeslot</t>
   </si>
   <si>
-    <t>Speaker prohibited timeslot tag</t>
+    <t>Speaker prohibited timeslot tags</t>
   </si>
   <si>
     <t>Hard penalty per prohibited tag in a talk's timeslot</t>
   </si>
   <si>
-    <t>Talk required timeslot tag</t>
-  </si>
-  <si>
-    <t>Talk prohibited timeslot tag</t>
-  </si>
-  <si>
-    <t>Speaker required room tag</t>
+    <t>Talk required timeslot tags</t>
+  </si>
+  <si>
+    <t>Talk prohibited timeslot tags</t>
+  </si>
+  <si>
+    <t>Speaker required room tags</t>
   </si>
   <si>
     <t>Hard penalty per missing required tag in a talk's room</t>
   </si>
   <si>
-    <t>Speaker prohibited room tag</t>
+    <t>Speaker prohibited room tags</t>
   </si>
   <si>
     <t>Hard penalty per prohibited tag in a talk's room</t>
   </si>
   <si>
-    <t>Talk required room tag</t>
-  </si>
-  <si>
-    <t>Talk prohibited room tag</t>
-  </si>
-  <si>
-    <t>Talk mutually-exclusive-talks tag</t>
+    <t>Talk required room tags</t>
+  </si>
+  <si>
+    <t>Talk prohibited room tags</t>
+  </si>
+  <si>
+    <t>Talk mutually-exclusive-talks tags</t>
   </si>
   <si>
     <t>Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>

</xml_diff>

<commit_message>
Rename numberOfLikes to favoriteCount
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -286,7 +286,7 @@
     <t>Popular talks</t>
   </si>
   <si>
-    <t>Soft penalty per 2 talks where the less popular one (has lower number of likes) is assigned a larger room than the more popular talk</t>
+    <t>Soft penalty per 2 talks where the less popular one (has lower favorite count) is assigned a larger room than the more popular talk</t>
   </si>
   <si>
     <t>Crowd control</t>
@@ -778,7 +778,7 @@
     <t>Prerequisite talks codes</t>
   </si>
   <si>
-    <t>Number of likes</t>
+    <t>Favorite count</t>
   </si>
   <si>
     <t>Crowd control risk</t>
@@ -10933,7 +10933,7 @@
     <col min="18" max="18" width="22.84375" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="31.2734375" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="26.23046875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.5390625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.25390625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="20.140625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.65234375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.14453125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Convert Talk mutually-exclusive-talks to a medium and soft constraint
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -295,6 +295,12 @@
     <t>Soft penalty per talks with crowd control risk greater than zero that are not in pairs</t>
   </si>
   <si>
+    <t>Talk mutually-exclusive-talks tags</t>
+  </si>
+  <si>
+    <t>Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
+  </si>
+  <si>
     <t>Talk type of timeslot</t>
   </si>
   <si>
@@ -365,12 +371,6 @@
   </si>
   <si>
     <t>Talk prohibited room tags</t>
-  </si>
-  <si>
-    <t>Talk mutually-exclusive-talks tags</t>
-  </si>
-  <si>
-    <t>Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
   </si>
   <si>
     <t>Talk prerequisite talks</t>
@@ -1952,7 +1952,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
@@ -2201,109 +2201,99 @@
         <v>39</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>10000.0</v>
+        <v>1.0</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
+    <row r="25"/>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>10000.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>10.0</v>
+        <v>10000.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>1.0</v>
+        <v>10000.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34">
@@ -2314,40 +2304,40 @@
         <v>1.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38">
@@ -2358,17 +2348,28 @@
         <v>1.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2383,7 +2384,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -2547,7 +2548,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -2771,7 +2772,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -2995,7 +2996,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -3219,7 +3220,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -3425,12 +3426,6 @@
       <c r="S3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>518</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells>
@@ -3449,50 +3444,58 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.0703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.73828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.15625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>535</v>
-      </c>
-    </row>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3502,7 +3505,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3.0" ySplit="1.0" state="frozen" topLeftCell="D2" activePane="bottomRight"/>
@@ -3849,7 +3852,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -4711,7 +4714,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AB74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -10904,7 +10907,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AB109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -20000,7 +20003,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
@@ -20105,7 +20108,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -20879,7 +20882,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -25311,7 +25314,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>

</xml_diff>

<commit_message>
Fix typo in configuration sheet
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/108talks-18timeslots-10rooms.xlsx
@@ -21,6 +21,9 @@
     <sheet name="Contents view" r:id="rId15" sheetId="13"/>
     <sheet name="Languages view" r:id="rId16" sheetId="14"/>
     <sheet name="Score view" r:id="rId17" sheetId="15"/>
+    <sheet name="Mon 2018-10-01" r:id="rId18" sheetId="16"/>
+    <sheet name="Tue 2018-10-02" r:id="rId19" sheetId="17"/>
+    <sheet name="Wed 2018-10-03" r:id="rId20" sheetId="18"/>
   </sheets>
 </workbook>
 </file>
@@ -33,11 +36,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -53,11 +55,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -73,11 +74,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -93,7 +93,26 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
+    Beth Smith, Amy Cole
+PINNED BY USER
+-10soft total
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0">
+      <text>
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
@@ -113,7 +132,7 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
@@ -133,21 +152,19 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
     <comment ref="C74" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -163,11 +180,10 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S098: Program flexible Spring
+        <t xml:space="preserve">S098-Mobile: Program flexible Spring
     Beth Smith, Amy Cole
 PINNED BY USER
 -10soft total
-    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -176,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6909" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6937" uniqueCount="539">
   <si>
     <t>Conference name</t>
   </si>
@@ -298,7 +314,7 @@
     <t>Talk mutually-exclusive-talks tags</t>
   </si>
   <si>
-    <t>Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
+    <t>Medium penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
   </si>
   <si>
     <t>Talk type of timeslot</t>
@@ -1791,6 +1807,10 @@
   </si>
   <si>
     <t xml:space="preserve">    S098</t>
+  </si>
+  <si>
+    <t>Program flexible Spring
+Beth Smith, Amy Cole</t>
   </si>
 </sst>
 </file>
@@ -1812,7 +1832,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1847,6 +1867,46 @@
         <fgColor rgb="FCAF3E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="8AE234"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FCE94F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="729FCF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E9B96E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="73D216"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EDD400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="3465A4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C17D11"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1860,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment wrapText="true" vertical="center"/>
@@ -1884,6 +1944,33 @@
       <alignment wrapText="true" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true">
       <alignment wrapText="true" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1915,6 +2002,18 @@
 </file>
 
 <file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
@@ -3496,6 +3595,203 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.94140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" ht="45.0" customHeight="true">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" ht="45.0" customHeight="true">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="4" ht="45.0" customHeight="true">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" ht="45.0" customHeight="true">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" ht="45.0" customHeight="true">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" ht="45.0" customHeight="true">
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.3515625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" ht="45.0" customHeight="true">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="45.0" customHeight="true">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" ht="45.0" customHeight="true">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" ht="45.0" customHeight="true">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" ht="45.0" customHeight="true">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" ht="45.0" customHeight="true">
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="18.12890625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" ht="45.0" customHeight="true">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="45.0" customHeight="true">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" ht="45.0" customHeight="true">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" ht="45.0" customHeight="true">
+      <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" ht="45.0" customHeight="true">
+      <c r="A6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" ht="45.0" customHeight="true">
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>